<commit_message>
added quiz marks of mat 101 section 4
</commit_message>
<xml_diff>
--- a/FALL 19/MAT 101/results_mat101_sec4.xlsx
+++ b/FALL 19/MAT 101/results_mat101_sec4.xlsx
@@ -1,27 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ulab_course_materials\FALL 19\MAT 101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C9A8AF-6667-45FF-8423-F7764C5A30C2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86551BA2-DB58-40E7-A894-302B70BBB3D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7308" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="quiz1" sheetId="1" r:id="rId1"/>
     <sheet name="mid" sheetId="2" r:id="rId2"/>
+    <sheet name="quiz2" sheetId="3" r:id="rId3"/>
+    <sheet name="quiz3" sheetId="4" r:id="rId4"/>
+    <sheet name="quiz_total" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="37">
   <si>
     <t>ID</t>
   </si>
@@ -118,12 +129,27 @@
   <si>
     <t>Marks 5</t>
   </si>
+  <si>
+    <t>Quiz 1</t>
+  </si>
+  <si>
+    <t>Quiz 2</t>
+  </si>
+  <si>
+    <t>Quiz 3</t>
+  </si>
+  <si>
+    <t>Quiz Total</t>
+  </si>
+  <si>
+    <t>Quiz Final</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -153,6 +179,10 @@
       <color theme="1"/>
       <name val="Cambria"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -202,7 +232,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="97">
+  <dxfs count="14">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -212,90 +242,6 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -369,58 +315,13 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <color rgb="FF00B050"/>
+        <color rgb="FF9C0006"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -454,61 +355,6 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -526,310 +372,6 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1048,7 +590,7 @@
   <dimension ref="A1:L48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="I2" sqref="I2:I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1123,11 +665,11 @@
         <v>6</v>
       </c>
       <c r="I2" s="7">
-        <f>C2+E2+G2</f>
+        <f t="shared" ref="I2:I17" si="0">C2+E2+G2</f>
         <v>9</v>
       </c>
       <c r="J2" s="7">
-        <f>D2+F2+H2</f>
+        <f t="shared" ref="J2:J17" si="1">D2+F2+H2</f>
         <v>20</v>
       </c>
       <c r="K2">
@@ -1159,19 +701,19 @@
         <v>6</v>
       </c>
       <c r="I3" s="7">
-        <f>C3+E3+G3</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J3" s="7">
-        <f>D3+F3+H3</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K17" si="0">(I3/J3)*100</f>
+        <f t="shared" ref="K3:K17" si="2">(I3/J3)*100</f>
         <v>0</v>
       </c>
       <c r="L3" s="9" t="str">
-        <f t="shared" ref="L3:L17" si="1">IF(K3&gt;94,"A+",IF(K3&gt;84,"A",IF(K3&gt;79,"A-",IF(K3&gt;74,"B+",IF(K3&gt;69,"B",IF(K3&gt;64,"B-",IF(K3&gt;59,"C+",IF(K3&gt;54,"C",IF(K3&gt;49,"D","F")))))))))</f>
+        <f t="shared" ref="L3:L17" si="3">IF(K3&gt;94,"A+",IF(K3&gt;84,"A",IF(K3&gt;79,"A-",IF(K3&gt;74,"B+",IF(K3&gt;69,"B",IF(K3&gt;64,"B-",IF(K3&gt;59,"C+",IF(K3&gt;54,"C",IF(K3&gt;49,"D","F")))))))))</f>
         <v>F</v>
       </c>
     </row>
@@ -1195,19 +737,19 @@
         <v>6</v>
       </c>
       <c r="I4" s="7">
-        <f>C4+E4+G4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J4" s="7">
-        <f>D4+F4+H4</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="K4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L4" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -1231,19 +773,19 @@
         <v>6</v>
       </c>
       <c r="I5" s="7">
-        <f>C5+E5+G5</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J5" s="7">
-        <f>D5+F5+H5</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="K5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L5" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -1273,19 +815,19 @@
         <v>6</v>
       </c>
       <c r="I6" s="7">
-        <f>C6+E6+G6</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="J6" s="7">
-        <f>D6+F6+H6</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="K6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>35</v>
       </c>
       <c r="L6" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -1309,19 +851,19 @@
         <v>6</v>
       </c>
       <c r="I7" s="7">
-        <f>C7+E7+G7</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J7" s="7">
-        <f>D7+F7+H7</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="K7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L7" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -1345,19 +887,19 @@
         <v>6</v>
       </c>
       <c r="I8" s="7">
-        <f>C8+E8+G8</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J8" s="7">
-        <f>D8+F8+H8</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="K8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L8" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -1381,19 +923,19 @@
         <v>6</v>
       </c>
       <c r="I9" s="7">
-        <f>C9+E9+G9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J9" s="7">
-        <f>D9+F9+H9</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="K9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L9" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -1423,19 +965,19 @@
         <v>6</v>
       </c>
       <c r="I10" s="7">
-        <f>C10+E10+G10</f>
+        <f t="shared" si="0"/>
         <v>14.5</v>
       </c>
       <c r="J10" s="7">
-        <f>D10+F10+H10</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="K10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>72.5</v>
       </c>
       <c r="L10" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>B</v>
       </c>
     </row>
@@ -1459,19 +1001,19 @@
         <v>6</v>
       </c>
       <c r="I11" s="7">
-        <f>C11+E11+G11</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J11" s="7">
-        <f>D11+F11+H11</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="K11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L11" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -1501,19 +1043,19 @@
         <v>6</v>
       </c>
       <c r="I12" s="7">
-        <f>C12+E12+G12</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="J12" s="7">
-        <f>D12+F12+H12</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="K12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>65</v>
       </c>
       <c r="L12" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>B-</v>
       </c>
     </row>
@@ -1537,19 +1079,19 @@
         <v>6</v>
       </c>
       <c r="I13" s="7">
-        <f>C13+E13+G13</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J13" s="7">
-        <f>D13+F13+H13</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="K13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L13" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -1579,19 +1121,19 @@
         <v>6</v>
       </c>
       <c r="I14" s="7">
-        <f>C14+E14+G14</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="J14" s="7">
-        <f>D14+F14+H14</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="K14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
       <c r="L14" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>C+</v>
       </c>
     </row>
@@ -1615,19 +1157,19 @@
         <v>6</v>
       </c>
       <c r="I15" s="7">
-        <f>C15+E15+G15</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J15" s="7">
-        <f>D15+F15+H15</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="K15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L15" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -1653,19 +1195,19 @@
         <v>6</v>
       </c>
       <c r="I16" s="7">
-        <f>C16+E16+G16</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J16" s="7">
-        <f>D16+F16+H16</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="K16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="L16" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -1695,19 +1237,19 @@
         <v>6</v>
       </c>
       <c r="I17" s="7">
-        <f>C17+E17+G17</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="J17" s="7">
-        <f>D17+F17+H17</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="K17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>55.000000000000007</v>
       </c>
       <c r="L17" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>C</v>
       </c>
     </row>
@@ -2085,17 +1627,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C17">
-    <cfRule type="cellIs" dxfId="15" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="greaterThan">
       <formula>$D$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E17">
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="greaterThan">
       <formula>$F$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G17">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="greaterThan">
       <formula>$H$2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2108,8 +1650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O1" sqref="O1:P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2204,11 +1746,11 @@
         <v>4</v>
       </c>
       <c r="M2" s="7">
-        <f>C2+E2+G2+I2+K2</f>
+        <f t="shared" ref="M2:M17" si="0">C2+E2+G2+I2+K2</f>
         <v>7</v>
       </c>
       <c r="N2" s="7">
-        <f>D2+F2+H2+J2+L2</f>
+        <f t="shared" ref="N2:N17" si="1">D2+F2+H2+J2+L2</f>
         <v>20</v>
       </c>
       <c r="O2">
@@ -2248,19 +1790,19 @@
         <v>4</v>
       </c>
       <c r="M3" s="7">
-        <f>C3+E3+G3+I3+K3</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N3" s="7">
-        <f>D3+F3+H3+J3+L3</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="O3">
-        <f t="shared" ref="O3:O17" si="0">(M3/N3)*100</f>
+        <f t="shared" ref="O3:O17" si="2">(M3/N3)*100</f>
         <v>0</v>
       </c>
       <c r="P3" s="9" t="str">
-        <f t="shared" ref="P3:P17" si="1">IF(O3&gt;94,"A+",IF(O3&gt;84,"A",IF(O3&gt;79,"A-",IF(O3&gt;74,"B+",IF(O3&gt;69,"B",IF(O3&gt;64,"B-",IF(O3&gt;59,"C+",IF(O3&gt;54,"C",IF(O3&gt;49,"D","F")))))))))</f>
+        <f t="shared" ref="P3:P17" si="3">IF(O3&gt;94,"A+",IF(O3&gt;84,"A",IF(O3&gt;79,"A-",IF(O3&gt;74,"B+",IF(O3&gt;69,"B",IF(O3&gt;64,"B-",IF(O3&gt;59,"C+",IF(O3&gt;54,"C",IF(O3&gt;49,"D","F")))))))))</f>
         <v>F</v>
       </c>
     </row>
@@ -2292,19 +1834,19 @@
         <v>4</v>
       </c>
       <c r="M4" s="7">
-        <f>C4+E4+G4+I4+K4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N4" s="7">
-        <f>D4+F4+H4+J4+L4</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="O4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P4" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -2336,19 +1878,19 @@
         <v>4</v>
       </c>
       <c r="M5" s="7">
-        <f>C5+E5+G5+I5+K5</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N5" s="7">
-        <f>D5+F5+H5+J5+L5</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="O5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P5" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -2384,19 +1926,19 @@
         <v>4</v>
       </c>
       <c r="M6" s="7">
-        <f>C6+E6+G6+I6+K6</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="N6" s="7">
-        <f>D6+F6+H6+J6+L6</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="O6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="P6" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -2432,19 +1974,19 @@
         <v>4</v>
       </c>
       <c r="M7" s="7">
-        <f>C7+E7+G7+I7+K7</f>
+        <f t="shared" si="0"/>
         <v>4.5</v>
       </c>
       <c r="N7" s="7">
-        <f>D7+F7+H7+J7+L7</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="O7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>22.5</v>
       </c>
       <c r="P7" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -2482,19 +2024,19 @@
         <v>4</v>
       </c>
       <c r="M8" s="7">
-        <f>C8+E8+G8+I8+K8</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="N8" s="7">
-        <f>D8+F8+H8+J8+L8</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="O8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>35</v>
       </c>
       <c r="P8" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -2526,19 +2068,19 @@
         <v>4</v>
       </c>
       <c r="M9" s="7">
-        <f>C9+E9+G9+I9+K9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N9" s="7">
-        <f>D9+F9+H9+J9+L9</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="O9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P9" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -2576,19 +2118,19 @@
         <v>4</v>
       </c>
       <c r="M10" s="7">
-        <f>C10+E10+G10+I10+K10</f>
+        <f t="shared" si="0"/>
         <v>6.5</v>
       </c>
       <c r="N10" s="7">
-        <f>D10+F10+H10+J10+L10</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="O10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>32.5</v>
       </c>
       <c r="P10" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -2624,19 +2166,19 @@
         <v>4</v>
       </c>
       <c r="M11" s="7">
-        <f>C11+E11+G11+I11+K11</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="N11" s="7">
-        <f>D11+F11+H11+J11+L11</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="O11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="P11" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -2678,19 +2220,19 @@
         <v>4</v>
       </c>
       <c r="M12" s="7">
-        <f>C12+E12+G12+I12+K12</f>
+        <f t="shared" si="0"/>
         <v>10.5</v>
       </c>
       <c r="N12" s="7">
-        <f>D12+F12+H12+J12+L12</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="O12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>52.5</v>
       </c>
       <c r="P12" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>D</v>
       </c>
     </row>
@@ -2722,19 +2264,19 @@
         <v>4</v>
       </c>
       <c r="M13" s="7">
-        <f>C13+E13+G13+I13+K13</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N13" s="7">
-        <f>D13+F13+H13+J13+L13</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="O13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P13" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -2770,19 +2312,19 @@
         <v>4</v>
       </c>
       <c r="M14" s="7">
-        <f>C14+E14+G14+I14+K14</f>
+        <f t="shared" si="0"/>
         <v>4.5</v>
       </c>
       <c r="N14" s="7">
-        <f>D14+F14+H14+J14+L14</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="O14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>22.5</v>
       </c>
       <c r="P14" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -2814,19 +2356,19 @@
         <v>4</v>
       </c>
       <c r="M15" s="7">
-        <f>C15+E15+G15+I15+K15</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N15" s="7">
-        <f>D15+F15+H15+J15+L15</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="O15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P15" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -2862,19 +2404,19 @@
         <v>4</v>
       </c>
       <c r="M16" s="7">
-        <f>C16+E16+G16+I16+K16</f>
+        <f t="shared" si="0"/>
         <v>4.5</v>
       </c>
       <c r="N16" s="7">
-        <f>D16+F16+H16+J16+L16</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="O16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>22.5</v>
       </c>
       <c r="P16" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -2912,48 +2454,1874 @@
         <v>4</v>
       </c>
       <c r="M17" s="7">
-        <f>C17+E17+G17+I17+K17</f>
+        <f t="shared" si="0"/>
         <v>10.5</v>
       </c>
       <c r="N17" s="7">
-        <f>D17+F17+H17+J17+L17</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="O17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>52.5</v>
       </c>
       <c r="P17" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>D</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C17">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="5" operator="greaterThan">
       <formula>$D$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E17">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="4" operator="greaterThan">
       <formula>$F$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G17">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="greaterThan">
       <formula>$H$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I17">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="greaterThan">
       <formula>$J$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K17">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="greaterThan">
       <formula>$L$2</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{082C1B9E-BEF4-4D2E-A59E-F7F0A8E0EE98}">
+  <dimension ref="A1:J17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.77734375" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" customWidth="1"/>
+    <col min="3" max="10" width="14.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="6">
+        <v>183011218</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="7">
+        <v>4</v>
+      </c>
+      <c r="D2" s="7">
+        <v>12</v>
+      </c>
+      <c r="E2" s="7">
+        <v>8</v>
+      </c>
+      <c r="F2" s="7">
+        <v>8</v>
+      </c>
+      <c r="G2" s="7">
+        <f>C2+E2</f>
+        <v>12</v>
+      </c>
+      <c r="H2" s="7">
+        <f>D2+F2</f>
+        <v>20</v>
+      </c>
+      <c r="I2">
+        <f>(G2/H2)*100</f>
+        <v>60</v>
+      </c>
+      <c r="J2" s="9" t="str">
+        <f>IF(I2&gt;94,"A+",IF(I2&gt;84,"A",IF(I2&gt;79,"A-",IF(I2&gt;74,"B+",IF(I2&gt;69,"B",IF(I2&gt;64,"B-",IF(I2&gt;59,"C+",IF(I2&gt;54,"C",IF(I2&gt;49,"D","F")))))))))</f>
+        <v>C+</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="6">
+        <v>173014033</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="7">
+        <v>12</v>
+      </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="7">
+        <v>8</v>
+      </c>
+      <c r="G3" s="7">
+        <f t="shared" ref="G3:G17" si="0">C3+E3</f>
+        <v>0</v>
+      </c>
+      <c r="H3" s="7">
+        <f t="shared" ref="H3:H17" si="1">D3+F3</f>
+        <v>20</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I17" si="2">(G3/H3)*100</f>
+        <v>0</v>
+      </c>
+      <c r="J3" s="9" t="str">
+        <f t="shared" ref="J3:J17" si="3">IF(I3&gt;94,"A+",IF(I3&gt;84,"A",IF(I3&gt;79,"A-",IF(I3&gt;74,"B+",IF(I3&gt;69,"B",IF(I3&gt;64,"B-",IF(I3&gt;59,"C+",IF(I3&gt;54,"C",IF(I3&gt;49,"D","F")))))))))</f>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="6">
+        <v>181014001</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7">
+        <v>12</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7">
+        <v>8</v>
+      </c>
+      <c r="G4" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H4" s="7">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J4" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
+        <v>181014051</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7">
+        <v>12</v>
+      </c>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7">
+        <v>8</v>
+      </c>
+      <c r="G5" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H5" s="7">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J5" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="6">
+        <v>181014126</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="7">
+        <v>12</v>
+      </c>
+      <c r="E6" s="8"/>
+      <c r="F6" s="7">
+        <v>8</v>
+      </c>
+      <c r="G6" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H6" s="7">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J6" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="6">
+        <v>182014056</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7">
+        <v>12</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7">
+        <v>8</v>
+      </c>
+      <c r="G7" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H7" s="7">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J7" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="6">
+        <v>183014070</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="7">
+        <v>4</v>
+      </c>
+      <c r="D8" s="7">
+        <v>12</v>
+      </c>
+      <c r="E8" s="7">
+        <v>6</v>
+      </c>
+      <c r="F8" s="7">
+        <v>8</v>
+      </c>
+      <c r="G8" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="H8" s="7">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="J8" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="6">
+        <v>191014032</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="7">
+        <v>12</v>
+      </c>
+      <c r="E9" s="8"/>
+      <c r="F9" s="7">
+        <v>8</v>
+      </c>
+      <c r="G9" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H9" s="7">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J9" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="6">
+        <v>193014009</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="7">
+        <v>2</v>
+      </c>
+      <c r="D10" s="7">
+        <v>12</v>
+      </c>
+      <c r="E10" s="7">
+        <v>8</v>
+      </c>
+      <c r="F10" s="7">
+        <v>8</v>
+      </c>
+      <c r="G10" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="H10" s="7">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="J10" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="6">
+        <v>193014067</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="7">
+        <v>2</v>
+      </c>
+      <c r="D11" s="7">
+        <v>12</v>
+      </c>
+      <c r="E11" s="7">
+        <v>2</v>
+      </c>
+      <c r="F11" s="7">
+        <v>8</v>
+      </c>
+      <c r="G11" s="7">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H11" s="7">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="J11" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="6">
+        <v>193014071</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="8">
+        <v>4</v>
+      </c>
+      <c r="D12" s="7">
+        <v>12</v>
+      </c>
+      <c r="E12" s="8">
+        <v>4</v>
+      </c>
+      <c r="F12" s="7">
+        <v>8</v>
+      </c>
+      <c r="G12" s="7">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H12" s="7">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="J12" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A13" s="6">
+        <v>193014072</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7">
+        <v>12</v>
+      </c>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7">
+        <v>8</v>
+      </c>
+      <c r="G13" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H13" s="7">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J13" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A14" s="6">
+        <v>193014073</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="7">
+        <v>2</v>
+      </c>
+      <c r="D14" s="7">
+        <v>12</v>
+      </c>
+      <c r="E14" s="7">
+        <v>2</v>
+      </c>
+      <c r="F14" s="7">
+        <v>8</v>
+      </c>
+      <c r="G14" s="7">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H14" s="7">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="J14" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A15" s="6">
+        <v>183016002</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7">
+        <v>12</v>
+      </c>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7">
+        <v>8</v>
+      </c>
+      <c r="G15" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H15" s="7">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J15" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A16" s="6">
+        <v>192016001</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="8"/>
+      <c r="D16" s="7">
+        <v>12</v>
+      </c>
+      <c r="E16" s="8"/>
+      <c r="F16" s="7">
+        <v>8</v>
+      </c>
+      <c r="G16" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H16" s="7">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J16" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A17" s="6">
+        <v>193016008</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="7">
+        <v>4</v>
+      </c>
+      <c r="D17" s="7">
+        <v>12</v>
+      </c>
+      <c r="E17" s="7">
+        <v>6</v>
+      </c>
+      <c r="F17" s="7">
+        <v>8</v>
+      </c>
+      <c r="G17" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="H17" s="7">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="J17" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>D</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C2:C17">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="greaterThan">
+      <formula>$D$2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E17">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="greaterThan">
+      <formula>$F$2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EAC316A-1F4D-4E67-A257-43105822BFCC}">
+  <dimension ref="A1:J17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.77734375" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" customWidth="1"/>
+    <col min="3" max="10" width="14.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="6">
+        <v>183011218</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="7">
+        <v>5</v>
+      </c>
+      <c r="D2" s="7">
+        <v>12</v>
+      </c>
+      <c r="E2" s="7">
+        <v>3</v>
+      </c>
+      <c r="F2" s="7">
+        <v>8</v>
+      </c>
+      <c r="G2" s="7">
+        <f>C2+E2</f>
+        <v>8</v>
+      </c>
+      <c r="H2" s="7">
+        <f>D2+F2</f>
+        <v>20</v>
+      </c>
+      <c r="I2">
+        <f>(G2/H2)*100</f>
+        <v>40</v>
+      </c>
+      <c r="J2" s="9" t="str">
+        <f>IF(I2&gt;94,"A+",IF(I2&gt;84,"A",IF(I2&gt;79,"A-",IF(I2&gt;74,"B+",IF(I2&gt;69,"B",IF(I2&gt;64,"B-",IF(I2&gt;59,"C+",IF(I2&gt;54,"C",IF(I2&gt;49,"D","F")))))))))</f>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="6">
+        <v>173014033</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="7">
+        <v>12</v>
+      </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="7">
+        <v>8</v>
+      </c>
+      <c r="G3" s="7">
+        <f t="shared" ref="G3:H17" si="0">C3+E3</f>
+        <v>0</v>
+      </c>
+      <c r="H3" s="7">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I17" si="1">(G3/H3)*100</f>
+        <v>0</v>
+      </c>
+      <c r="J3" s="9" t="str">
+        <f t="shared" ref="J3:J17" si="2">IF(I3&gt;94,"A+",IF(I3&gt;84,"A",IF(I3&gt;79,"A-",IF(I3&gt;74,"B+",IF(I3&gt;69,"B",IF(I3&gt;64,"B-",IF(I3&gt;59,"C+",IF(I3&gt;54,"C",IF(I3&gt;49,"D","F")))))))))</f>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="6">
+        <v>181014001</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7">
+        <v>12</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7">
+        <v>8</v>
+      </c>
+      <c r="G4" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H4" s="7">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J4" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
+        <v>181014051</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7">
+        <v>12</v>
+      </c>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7">
+        <v>8</v>
+      </c>
+      <c r="G5" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H5" s="7">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J5" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="6">
+        <v>181014126</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="7">
+        <v>12</v>
+      </c>
+      <c r="E6" s="8"/>
+      <c r="F6" s="7">
+        <v>8</v>
+      </c>
+      <c r="G6" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H6" s="7">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J6" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="6">
+        <v>182014056</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="7">
+        <v>6</v>
+      </c>
+      <c r="D7" s="7">
+        <v>12</v>
+      </c>
+      <c r="E7" s="7">
+        <v>2</v>
+      </c>
+      <c r="F7" s="7">
+        <v>8</v>
+      </c>
+      <c r="G7" s="7">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H7" s="7">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="J7" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="6">
+        <v>183014070</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7">
+        <v>12</v>
+      </c>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7">
+        <v>8</v>
+      </c>
+      <c r="G8" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H8" s="7">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J8" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="6">
+        <v>191014032</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="7">
+        <v>12</v>
+      </c>
+      <c r="E9" s="8"/>
+      <c r="F9" s="7">
+        <v>8</v>
+      </c>
+      <c r="G9" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H9" s="7">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J9" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="6">
+        <v>193014009</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7">
+        <v>12</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7">
+        <v>8</v>
+      </c>
+      <c r="G10" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="7">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J10" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="6">
+        <v>193014067</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7">
+        <v>12</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7">
+        <v>8</v>
+      </c>
+      <c r="G11" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H11" s="7">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J11" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="6">
+        <v>193014071</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="8">
+        <v>12</v>
+      </c>
+      <c r="D12" s="7">
+        <v>12</v>
+      </c>
+      <c r="E12" s="8">
+        <v>2</v>
+      </c>
+      <c r="F12" s="7">
+        <v>8</v>
+      </c>
+      <c r="G12" s="7">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="H12" s="7">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="J12" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A13" s="6">
+        <v>193014072</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7">
+        <v>12</v>
+      </c>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7">
+        <v>8</v>
+      </c>
+      <c r="G13" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H13" s="7">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J13" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A14" s="6">
+        <v>193014073</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7">
+        <v>12</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7">
+        <v>8</v>
+      </c>
+      <c r="G14" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H14" s="7">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J14" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A15" s="6">
+        <v>183016002</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7">
+        <v>12</v>
+      </c>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7">
+        <v>8</v>
+      </c>
+      <c r="G15" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H15" s="7">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J15" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A16" s="6">
+        <v>192016001</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="8">
+        <v>6</v>
+      </c>
+      <c r="D16" s="7">
+        <v>12</v>
+      </c>
+      <c r="E16" s="8">
+        <v>2</v>
+      </c>
+      <c r="F16" s="7">
+        <v>8</v>
+      </c>
+      <c r="G16" s="7">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H16" s="7">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="J16" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A17" s="6">
+        <v>193016008</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="7">
+        <v>5</v>
+      </c>
+      <c r="D17" s="7">
+        <v>12</v>
+      </c>
+      <c r="E17" s="7">
+        <v>4</v>
+      </c>
+      <c r="F17" s="7">
+        <v>8</v>
+      </c>
+      <c r="G17" s="7">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="H17" s="7">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="J17" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E2:E17">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+      <formula>$F$2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C17">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+      <formula>$D$2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2461B99B-E650-4F8E-B1A3-A4187F7BFC8C}">
+  <dimension ref="A1:J17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.77734375" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" customWidth="1"/>
+    <col min="3" max="7" width="14.77734375" customWidth="1"/>
+    <col min="8" max="10" width="14.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="6">
+        <v>183011218</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>9</v>
+      </c>
+      <c r="D2">
+        <v>12</v>
+      </c>
+      <c r="E2">
+        <v>8</v>
+      </c>
+      <c r="F2">
+        <f>LARGE(C2:E2,1)+LARGE(C2:E2,2)</f>
+        <v>21</v>
+      </c>
+      <c r="G2">
+        <f>F2/4</f>
+        <v>5.25</v>
+      </c>
+      <c r="H2">
+        <v>10</v>
+      </c>
+      <c r="I2">
+        <f>(G2/H2)*100</f>
+        <v>52.5</v>
+      </c>
+      <c r="J2" s="9" t="str">
+        <f>IF(I2&gt;94,"A+",IF(I2&gt;84,"A",IF(I2&gt;79,"A-",IF(I2&gt;74,"B+",IF(I2&gt;69,"B",IF(I2&gt;64,"B-",IF(I2&gt;59,"C+",IF(I2&gt;54,"C",IF(I2&gt;49,"D","F")))))))))</f>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="6">
+        <v>173014033</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F17" si="0">LARGE(C3:E3,1)+LARGE(C3:E3,2)</f>
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G17" si="1">F3/4</f>
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>10</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I17" si="2">(G3/H3)*100</f>
+        <v>0</v>
+      </c>
+      <c r="J3" s="9" t="str">
+        <f t="shared" ref="J3:J17" si="3">IF(I3&gt;94,"A+",IF(I3&gt;84,"A",IF(I3&gt;79,"A-",IF(I3&gt;74,"B+",IF(I3&gt;69,"B",IF(I3&gt;64,"B-",IF(I3&gt;59,"C+",IF(I3&gt;54,"C",IF(I3&gt;49,"D","F")))))))))</f>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="6">
+        <v>181014001</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>10</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J4" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
+        <v>181014051</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>10</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J5" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="6">
+        <v>181014126</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>1.75</v>
+      </c>
+      <c r="H6">
+        <v>10</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="2"/>
+        <v>17.5</v>
+      </c>
+      <c r="J6" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="6">
+        <v>182014056</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>8</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="H7">
+        <v>10</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="J7" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="6">
+        <v>183014070</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="H8">
+        <v>10</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="J8" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="6">
+        <v>191014032</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>10</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J9" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="6">
+        <v>193014009</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10">
+        <v>14.5</v>
+      </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>24.5</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>6.125</v>
+      </c>
+      <c r="H10">
+        <v>10</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="2"/>
+        <v>61.250000000000007</v>
+      </c>
+      <c r="J10" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>C+</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="6">
+        <v>193014067</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>10</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="J11" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="6">
+        <v>193014071</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12">
+        <v>13</v>
+      </c>
+      <c r="D12">
+        <v>8</v>
+      </c>
+      <c r="E12">
+        <v>14</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>6.75</v>
+      </c>
+      <c r="H12">
+        <v>10</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="2"/>
+        <v>67.5</v>
+      </c>
+      <c r="J12" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>B-</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A13" s="6">
+        <v>193014072</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>10</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J13" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A14" s="6">
+        <v>193014073</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14">
+        <v>12</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="H14">
+        <v>10</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="J14" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A15" s="6">
+        <v>183016002</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>10</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J15" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A16" s="6">
+        <v>192016001</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>8</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="1"/>
+        <v>2.25</v>
+      </c>
+      <c r="H16">
+        <v>10</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="2"/>
+        <v>22.5</v>
+      </c>
+      <c r="J16" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A17" s="6">
+        <v>193016008</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17">
+        <v>11</v>
+      </c>
+      <c r="D17">
+        <v>10</v>
+      </c>
+      <c r="E17">
+        <v>9</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>5.25</v>
+      </c>
+      <c r="H17">
+        <v>10</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="2"/>
+        <v>52.5</v>
+      </c>
+      <c r="J17" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>D</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added attendance for mat 101 section 4
</commit_message>
<xml_diff>
--- a/FALL 19/MAT 101/results_mat101_sec4.xlsx
+++ b/FALL 19/MAT 101/results_mat101_sec4.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ulab_course_materials\FALL 19\MAT 101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3013559A-54E1-4ABC-ADD2-B6F3E540BAA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC141D3B-6475-40DD-BA2E-2F8C8DFC1D5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="quiz1" sheetId="1" r:id="rId1"/>
-    <sheet name="quiz2" sheetId="3" r:id="rId2"/>
-    <sheet name="quiz3" sheetId="4" r:id="rId3"/>
-    <sheet name="quiz_total" sheetId="5" r:id="rId4"/>
-    <sheet name="mid" sheetId="2" r:id="rId5"/>
-    <sheet name="final" sheetId="6" r:id="rId6"/>
+    <sheet name="attendance" sheetId="7" r:id="rId1"/>
+    <sheet name="quiz1" sheetId="1" r:id="rId2"/>
+    <sheet name="quiz2" sheetId="3" r:id="rId3"/>
+    <sheet name="quiz3" sheetId="4" r:id="rId4"/>
+    <sheet name="quiz_total" sheetId="5" r:id="rId5"/>
+    <sheet name="mid" sheetId="2" r:id="rId6"/>
+    <sheet name="final" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="41">
   <si>
     <t>ID</t>
   </si>
@@ -151,12 +152,18 @@
   <si>
     <t>Marks 6</t>
   </si>
+  <si>
+    <t>Absent</t>
+  </si>
+  <si>
+    <t>Present</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -191,6 +198,12 @@
       <sz val="8"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -200,7 +213,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -208,11 +221,91 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -235,11 +328,67 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="19">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -620,6 +769,547 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97BD6406-ADEC-4F97-961E-16D0039E8A9F}">
+  <dimension ref="A1:H18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" customWidth="1"/>
+    <col min="3" max="8" width="14.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="14">
+        <v>183011218</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="16">
+        <v>19</v>
+      </c>
+      <c r="D2" s="16">
+        <v>2</v>
+      </c>
+      <c r="E2" s="16">
+        <f>C2-D2</f>
+        <v>17</v>
+      </c>
+      <c r="F2" s="16">
+        <f>ROUNDUP((E2/C2)*F$18,0)</f>
+        <v>9</v>
+      </c>
+      <c r="G2" s="17">
+        <f>(F2/F$18)*100</f>
+        <v>90</v>
+      </c>
+      <c r="H2" s="13" t="str">
+        <f>IF(G2&gt;94,"A+",IF(G2&gt;84,"A",IF(G2&gt;79,"A-",IF(G2&gt;74,"B+",IF(G2&gt;69,"B",IF(G2&gt;64,"B-",IF(G2&gt;59,"C+",IF(G2&gt;54,"C",IF(G2&gt;49,"D","F")))))))))</f>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="14">
+        <v>173014033</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="16">
+        <v>19</v>
+      </c>
+      <c r="D3" s="18">
+        <v>14</v>
+      </c>
+      <c r="E3" s="16">
+        <f t="shared" ref="E3:E17" si="0">C3-D3</f>
+        <v>5</v>
+      </c>
+      <c r="F3" s="16">
+        <f t="shared" ref="F3:F17" si="1">ROUNDUP((E3/C3)*F$18,0)</f>
+        <v>3</v>
+      </c>
+      <c r="G3" s="17">
+        <f t="shared" ref="G3:G17" si="2">(F3/F$18)*100</f>
+        <v>30</v>
+      </c>
+      <c r="H3" s="13" t="str">
+        <f t="shared" ref="H3:H17" si="3">IF(G3&gt;94,"A+",IF(G3&gt;84,"A",IF(G3&gt;79,"A-",IF(G3&gt;74,"B+",IF(G3&gt;69,"B",IF(G3&gt;64,"B-",IF(G3&gt;59,"C+",IF(G3&gt;54,"C",IF(G3&gt;49,"D","F")))))))))</f>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="14">
+        <v>181014001</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="16">
+        <v>19</v>
+      </c>
+      <c r="D4" s="18">
+        <v>17</v>
+      </c>
+      <c r="E4" s="16">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F4" s="16">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G4" s="17">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="H4" s="13" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="14">
+        <v>181014051</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="16">
+        <v>19</v>
+      </c>
+      <c r="D5" s="18">
+        <v>17</v>
+      </c>
+      <c r="E5" s="16">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F5" s="16">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G5" s="17">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="H5" s="13" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="14">
+        <v>181014126</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="16">
+        <v>19</v>
+      </c>
+      <c r="D6" s="25">
+        <v>7</v>
+      </c>
+      <c r="E6" s="16">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="F6" s="16">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="G6" s="17">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="H6" s="13" t="str">
+        <f t="shared" si="3"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="14">
+        <v>182014056</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="16">
+        <v>19</v>
+      </c>
+      <c r="D7" s="25">
+        <v>7</v>
+      </c>
+      <c r="E7" s="16">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="F7" s="16">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="G7" s="17">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="H7" s="13" t="str">
+        <f t="shared" si="3"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="14">
+        <v>183014070</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="16">
+        <v>19</v>
+      </c>
+      <c r="D8" s="25">
+        <v>12</v>
+      </c>
+      <c r="E8" s="16">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="F8" s="16">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="G8" s="17">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="H8" s="13" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="14">
+        <v>191014032</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="16">
+        <v>19</v>
+      </c>
+      <c r="D9" s="25">
+        <v>17</v>
+      </c>
+      <c r="E9" s="16">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F9" s="16">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G9" s="17">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="H9" s="13" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="14">
+        <v>193014009</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="16">
+        <v>19</v>
+      </c>
+      <c r="D10" s="25">
+        <v>1</v>
+      </c>
+      <c r="E10" s="16">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="F10" s="16">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="G10" s="17">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="H10" s="13" t="str">
+        <f t="shared" si="3"/>
+        <v>A+</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="14">
+        <v>193014067</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="16">
+        <v>19</v>
+      </c>
+      <c r="D11" s="25">
+        <v>7</v>
+      </c>
+      <c r="E11" s="16">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="F11" s="16">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="G11" s="17">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="H11" s="13" t="str">
+        <f t="shared" si="3"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="14">
+        <v>193014071</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="16">
+        <v>19</v>
+      </c>
+      <c r="D12" s="25">
+        <v>1</v>
+      </c>
+      <c r="E12" s="16">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="F12" s="16">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="G12" s="17">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="H12" s="13" t="str">
+        <f t="shared" si="3"/>
+        <v>A+</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A13" s="14">
+        <v>193014072</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="16">
+        <v>19</v>
+      </c>
+      <c r="D13" s="25">
+        <v>17</v>
+      </c>
+      <c r="E13" s="16">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F13" s="16">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G13" s="17">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="H13" s="13" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A14" s="14">
+        <v>193014073</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="16">
+        <v>19</v>
+      </c>
+      <c r="D14" s="25">
+        <v>3</v>
+      </c>
+      <c r="E14" s="16">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="F14" s="16">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="G14" s="17">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="H14" s="13" t="str">
+        <f t="shared" si="3"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A15" s="14">
+        <v>183016002</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="16">
+        <v>19</v>
+      </c>
+      <c r="D15" s="18">
+        <v>17</v>
+      </c>
+      <c r="E15" s="16">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F15" s="16">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G15" s="17">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="H15" s="13" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A16" s="14">
+        <v>192016001</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="16">
+        <v>19</v>
+      </c>
+      <c r="D16" s="18">
+        <v>10</v>
+      </c>
+      <c r="E16" s="16">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="F16" s="16">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="G16" s="17">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="H16" s="13" t="str">
+        <f t="shared" si="3"/>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="19">
+        <v>193016008</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="22">
+        <v>19</v>
+      </c>
+      <c r="D17" s="21">
+        <v>6</v>
+      </c>
+      <c r="E17" s="22">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="F17" s="22">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="G17" s="23">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="H17" s="24" t="str">
+        <f t="shared" si="3"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C2:E2 E3:E17 C3:C17">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H17">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -627,7 +1317,7 @@
   <dimension ref="A1:L48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I17"/>
+      <selection activeCell="A2" sqref="A2:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1664,17 +2354,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C17">
-    <cfRule type="cellIs" dxfId="16" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="3" operator="greaterThan">
       <formula>$D$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E17">
-    <cfRule type="cellIs" dxfId="15" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="2" operator="greaterThan">
       <formula>$F$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G17">
-    <cfRule type="cellIs" dxfId="14" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="1" operator="greaterThan">
       <formula>$H$2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1683,7 +2373,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{082C1B9E-BEF4-4D2E-A59E-F7F0A8E0EE98}">
   <dimension ref="A1:J17"/>
   <sheetViews>
@@ -2272,12 +2962,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C17">
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="3" operator="greaterThan">
       <formula>$D$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E17">
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="greaterThan">
       <formula>$F$2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2285,7 +2975,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EAC316A-1F4D-4E67-A257-43105822BFCC}">
   <dimension ref="A1:J17"/>
   <sheetViews>
@@ -2866,12 +3556,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E17">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="greaterThan">
       <formula>$F$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C17">
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="greaterThan">
       <formula>$D$2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2879,7 +3569,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2461B99B-E650-4F8E-B1A3-A4187F7BFC8C}">
   <dimension ref="A1:J17"/>
   <sheetViews>
@@ -3509,7 +4199,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P17"/>
   <sheetViews>
@@ -4335,27 +5025,27 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C17">
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="5" operator="greaterThan">
       <formula>$D$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E17">
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="4" operator="greaterThan">
       <formula>$F$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G17">
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="greaterThan">
       <formula>$H$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I17">
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="greaterThan">
       <formula>$J$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K17">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="greaterThan">
       <formula>$L$2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4363,11 +5053,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01230E4E-9F21-464B-AB8D-C05858C1812B}">
   <dimension ref="A1:R19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
@@ -5308,27 +5998,27 @@
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="C2:C17">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="greaterThan">
       <formula>$D$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E17">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="greaterThan">
       <formula>$F$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G17">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="greaterThan">
       <formula>$H$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I17">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
       <formula>$J$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K17">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
       <formula>$L$2</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
added attendance and project marks for cse 208 section 2 and cse 104 section 1. also added assignment marks for mat 101
</commit_message>
<xml_diff>
--- a/FALL 19/MAT 101/results_mat101_sec4.xlsx
+++ b/FALL 19/MAT 101/results_mat101_sec4.xlsx
@@ -1,27 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ulab_course_materials\FALL 19\MAT 101\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC141D3B-6475-40DD-BA2E-2F8C8DFC1D5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="21840" windowHeight="13740" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="attendance" sheetId="7" r:id="rId1"/>
-    <sheet name="quiz1" sheetId="1" r:id="rId2"/>
-    <sheet name="quiz2" sheetId="3" r:id="rId3"/>
-    <sheet name="quiz3" sheetId="4" r:id="rId4"/>
-    <sheet name="quiz_total" sheetId="5" r:id="rId5"/>
-    <sheet name="mid" sheetId="2" r:id="rId6"/>
-    <sheet name="final" sheetId="6" r:id="rId7"/>
+    <sheet name="assignments" sheetId="8" r:id="rId2"/>
+    <sheet name="quiz1" sheetId="1" r:id="rId3"/>
+    <sheet name="quiz2" sheetId="3" r:id="rId4"/>
+    <sheet name="quiz3" sheetId="4" r:id="rId5"/>
+    <sheet name="quiz_total" sheetId="5" r:id="rId6"/>
+    <sheet name="mid" sheetId="2" r:id="rId7"/>
+    <sheet name="final" sheetId="6" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -34,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="41">
   <si>
     <t>ID</t>
   </si>
@@ -162,8 +157,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -366,11 +361,9 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="20">
     <dxf>
       <font>
-        <condense val="0"/>
-        <extend val="0"/>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -541,6 +534,20 @@
     </dxf>
     <dxf>
       <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -769,21 +776,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97BD6406-ADEC-4F97-961E-16D0039E8A9F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" customWidth="1"/>
-    <col min="3" max="8" width="14.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="8" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -809,7 +816,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="15">
       <c r="A2" s="14">
         <v>183011218</v>
       </c>
@@ -839,7 +846,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="15">
       <c r="A3" s="14">
         <v>173014033</v>
       </c>
@@ -869,7 +876,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="15">
       <c r="A4" s="14">
         <v>181014001</v>
       </c>
@@ -899,7 +906,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="15">
       <c r="A5" s="14">
         <v>181014051</v>
       </c>
@@ -929,7 +936,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="15">
       <c r="A6" s="14">
         <v>181014126</v>
       </c>
@@ -959,7 +966,7 @@
         <v>B</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="15">
       <c r="A7" s="14">
         <v>182014056</v>
       </c>
@@ -989,7 +996,7 @@
         <v>B</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="15">
       <c r="A8" s="14">
         <v>183014070</v>
       </c>
@@ -1019,7 +1026,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="15">
       <c r="A9" s="14">
         <v>191014032</v>
       </c>
@@ -1049,7 +1056,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="15">
       <c r="A10" s="14">
         <v>193014009</v>
       </c>
@@ -1079,7 +1086,7 @@
         <v>A+</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="15">
       <c r="A11" s="14">
         <v>193014067</v>
       </c>
@@ -1109,7 +1116,7 @@
         <v>B</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="15">
       <c r="A12" s="14">
         <v>193014071</v>
       </c>
@@ -1139,7 +1146,7 @@
         <v>A+</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="15">
       <c r="A13" s="14">
         <v>193014072</v>
       </c>
@@ -1169,7 +1176,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="15">
       <c r="A14" s="14">
         <v>193014073</v>
       </c>
@@ -1199,7 +1206,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="15">
       <c r="A15" s="14">
         <v>183016002</v>
       </c>
@@ -1229,7 +1236,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="15">
       <c r="A16" s="14">
         <v>192016001</v>
       </c>
@@ -1259,7 +1266,7 @@
         <v>D</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" ht="15.75" thickBot="1">
       <c r="A17" s="19">
         <v>193016008</v>
       </c>
@@ -1289,19 +1296,19 @@
         <v>B</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="F18">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:E2 E3:E17 C3:C17">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="2" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H17">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="1" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1310,7 +1317,358 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="5" width="14.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15">
+      <c r="A2" s="14">
+        <v>183011218</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="16">
+        <v>9</v>
+      </c>
+      <c r="D2" s="17">
+        <f>(C2/C$18)*100</f>
+        <v>90</v>
+      </c>
+      <c r="E2" s="13" t="str">
+        <f>IF(D2&gt;94,"A+",IF(D2&gt;84,"A",IF(D2&gt;79,"A-",IF(D2&gt;74,"B+",IF(D2&gt;69,"B",IF(D2&gt;64,"B-",IF(D2&gt;59,"C+",IF(D2&gt;54,"C",IF(D2&gt;49,"D","F")))))))))</f>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15">
+      <c r="A3" s="14">
+        <v>173014033</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="16">
+        <v>0</v>
+      </c>
+      <c r="D3" s="17">
+        <f t="shared" ref="D3:D17" si="0">(C3/C$18)*100</f>
+        <v>0</v>
+      </c>
+      <c r="E3" s="13" t="str">
+        <f t="shared" ref="E3:E17" si="1">IF(D3&gt;94,"A+",IF(D3&gt;84,"A",IF(D3&gt;79,"A-",IF(D3&gt;74,"B+",IF(D3&gt;69,"B",IF(D3&gt;64,"B-",IF(D3&gt;59,"C+",IF(D3&gt;54,"C",IF(D3&gt;49,"D","F")))))))))</f>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15">
+      <c r="A4" s="14">
+        <v>181014001</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="16">
+        <v>0</v>
+      </c>
+      <c r="D4" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E4" s="13" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15">
+      <c r="A5" s="14">
+        <v>181014051</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="16">
+        <v>0</v>
+      </c>
+      <c r="D5" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E5" s="13" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15">
+      <c r="A6" s="14">
+        <v>181014126</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="16">
+        <v>8</v>
+      </c>
+      <c r="D6" s="17">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="E6" s="13" t="str">
+        <f t="shared" si="1"/>
+        <v>A-</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15">
+      <c r="A7" s="14">
+        <v>182014056</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="16">
+        <v>8</v>
+      </c>
+      <c r="D7" s="17">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="E7" s="13" t="str">
+        <f t="shared" si="1"/>
+        <v>A-</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15">
+      <c r="A8" s="14">
+        <v>183014070</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="16">
+        <v>0</v>
+      </c>
+      <c r="D8" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E8" s="13" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15">
+      <c r="A9" s="14">
+        <v>191014032</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="16">
+        <v>0</v>
+      </c>
+      <c r="D9" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E9" s="13" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15">
+      <c r="A10" s="14">
+        <v>193014009</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="16">
+        <v>10</v>
+      </c>
+      <c r="D10" s="17">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="E10" s="13" t="str">
+        <f t="shared" si="1"/>
+        <v>A+</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15">
+      <c r="A11" s="14">
+        <v>193014067</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="16">
+        <v>8</v>
+      </c>
+      <c r="D11" s="17">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="E11" s="13" t="str">
+        <f t="shared" si="1"/>
+        <v>A-</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15">
+      <c r="A12" s="14">
+        <v>193014071</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="16">
+        <v>10</v>
+      </c>
+      <c r="D12" s="17">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="E12" s="13" t="str">
+        <f t="shared" si="1"/>
+        <v>A+</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15">
+      <c r="A13" s="14">
+        <v>193014072</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="16">
+        <v>0</v>
+      </c>
+      <c r="D13" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E13" s="13" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15">
+      <c r="A14" s="14">
+        <v>193014073</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="16">
+        <v>10</v>
+      </c>
+      <c r="D14" s="17">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="E14" s="13" t="str">
+        <f t="shared" si="1"/>
+        <v>A+</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15">
+      <c r="A15" s="14">
+        <v>183016002</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="16">
+        <v>0</v>
+      </c>
+      <c r="D15" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E15" s="13" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15">
+      <c r="A16" s="14">
+        <v>192016001</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="16">
+        <v>9</v>
+      </c>
+      <c r="D16" s="17">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+      <c r="E16" s="13" t="str">
+        <f t="shared" si="1"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A17" s="19">
+        <v>193016008</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="22">
+        <v>8</v>
+      </c>
+      <c r="D17" s="23">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="E17" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>A-</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="C18">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E2:E17">
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -1320,15 +1678,15 @@
       <selection activeCell="A2" sqref="A2:B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" style="2" customWidth="1"/>
-    <col min="3" max="10" width="14.6640625" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="14.44140625" style="2"/>
+    <col min="1" max="1" width="14.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" style="2" customWidth="1"/>
+    <col min="3" max="10" width="14.7109375" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="14.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15.95" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1366,7 +1724,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="15" customHeight="1">
       <c r="A2" s="6">
         <v>183011218</v>
       </c>
@@ -1408,7 +1766,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="15" customHeight="1">
       <c r="A3" s="6">
         <v>173014033</v>
       </c>
@@ -1444,7 +1802,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="15" customHeight="1">
       <c r="A4" s="6">
         <v>181014001</v>
       </c>
@@ -1480,7 +1838,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="15" customHeight="1">
       <c r="A5" s="6">
         <v>181014051</v>
       </c>
@@ -1516,7 +1874,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="15" customHeight="1">
       <c r="A6" s="6">
         <v>181014126</v>
       </c>
@@ -1558,7 +1916,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="15" customHeight="1">
       <c r="A7" s="6">
         <v>182014056</v>
       </c>
@@ -1594,7 +1952,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="15" customHeight="1">
       <c r="A8" s="6">
         <v>183014070</v>
       </c>
@@ -1630,7 +1988,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="15" customHeight="1">
       <c r="A9" s="6">
         <v>191014032</v>
       </c>
@@ -1666,7 +2024,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="15" customHeight="1">
       <c r="A10" s="6">
         <v>193014009</v>
       </c>
@@ -1708,7 +2066,7 @@
         <v>B</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="15" customHeight="1">
       <c r="A11" s="6">
         <v>193014067</v>
       </c>
@@ -1744,7 +2102,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="15" customHeight="1">
       <c r="A12" s="6">
         <v>193014071</v>
       </c>
@@ -1786,7 +2144,7 @@
         <v>B-</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="15" customHeight="1">
       <c r="A13" s="6">
         <v>193014072</v>
       </c>
@@ -1822,7 +2180,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="15" customHeight="1">
       <c r="A14" s="6">
         <v>193014073</v>
       </c>
@@ -1864,7 +2222,7 @@
         <v>C+</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="15" customHeight="1">
       <c r="A15" s="6">
         <v>183016002</v>
       </c>
@@ -1900,7 +2258,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="15" customHeight="1">
       <c r="A16" s="6">
         <v>192016001</v>
       </c>
@@ -1938,7 +2296,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="15" customHeight="1">
       <c r="A17" s="6">
         <v>193016008</v>
       </c>
@@ -1980,7 +2338,7 @@
         <v>C</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="15">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="5"/>
@@ -1992,7 +2350,7 @@
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
     </row>
-    <row r="19" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="15">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="4"/>
@@ -2004,7 +2362,7 @@
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
     </row>
-    <row r="20" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="15">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="4"/>
@@ -2016,7 +2374,7 @@
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
     </row>
-    <row r="21" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="15">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="4"/>
@@ -2028,7 +2386,7 @@
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
     </row>
-    <row r="22" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" ht="15">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="4"/>
@@ -2040,7 +2398,7 @@
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
     </row>
-    <row r="23" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" ht="15">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="4"/>
@@ -2052,7 +2410,7 @@
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
     </row>
-    <row r="24" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" ht="15">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="4"/>
@@ -2064,7 +2422,7 @@
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
     </row>
-    <row r="25" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" ht="15">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="5"/>
@@ -2076,7 +2434,7 @@
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
     </row>
-    <row r="26" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" ht="15">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="5"/>
@@ -2088,7 +2446,7 @@
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
     </row>
-    <row r="27" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" ht="15">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="4"/>
@@ -2100,7 +2458,7 @@
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
     </row>
-    <row r="28" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" ht="15">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="4"/>
@@ -2112,7 +2470,7 @@
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
     </row>
-    <row r="29" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" ht="15">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="4"/>
@@ -2124,7 +2482,7 @@
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
     </row>
-    <row r="30" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" ht="15">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="5"/>
@@ -2136,7 +2494,7 @@
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
     </row>
-    <row r="31" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" ht="15">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="4"/>
@@ -2148,7 +2506,7 @@
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
     </row>
-    <row r="32" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" ht="15">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="4"/>
@@ -2160,7 +2518,7 @@
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
     </row>
-    <row r="33" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" ht="15">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="4"/>
@@ -2172,7 +2530,7 @@
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
     </row>
-    <row r="34" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" ht="15">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="4"/>
@@ -2184,7 +2542,7 @@
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
     </row>
-    <row r="35" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" ht="15">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="4"/>
@@ -2196,7 +2554,7 @@
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
     </row>
-    <row r="36" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" ht="15">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="4"/>
@@ -2208,7 +2566,7 @@
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
     </row>
-    <row r="37" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" ht="15">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="4"/>
@@ -2220,7 +2578,7 @@
       <c r="I37" s="4"/>
       <c r="J37" s="4"/>
     </row>
-    <row r="38" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" ht="15">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="4"/>
@@ -2232,7 +2590,7 @@
       <c r="I38" s="4"/>
       <c r="J38" s="4"/>
     </row>
-    <row r="39" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" ht="15">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="4"/>
@@ -2244,7 +2602,7 @@
       <c r="I39" s="4"/>
       <c r="J39" s="4"/>
     </row>
-    <row r="40" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" ht="15">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="4"/>
@@ -2256,7 +2614,7 @@
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
     </row>
-    <row r="41" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" ht="15">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="4"/>
@@ -2268,7 +2626,7 @@
       <c r="I41" s="4"/>
       <c r="J41" s="4"/>
     </row>
-    <row r="42" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" ht="15">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="4"/>
@@ -2280,7 +2638,7 @@
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
     </row>
-    <row r="43" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" ht="15">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="4"/>
@@ -2292,7 +2650,7 @@
       <c r="I43" s="4"/>
       <c r="J43" s="4"/>
     </row>
-    <row r="44" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" ht="15">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="4"/>
@@ -2304,7 +2662,7 @@
       <c r="I44" s="4"/>
       <c r="J44" s="4"/>
     </row>
-    <row r="45" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" ht="15">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="4"/>
@@ -2316,7 +2674,7 @@
       <c r="I45" s="4"/>
       <c r="J45" s="4"/>
     </row>
-    <row r="46" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" ht="15">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="4"/>
@@ -2328,7 +2686,7 @@
       <c r="I46" s="4"/>
       <c r="J46" s="4"/>
     </row>
-    <row r="47" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" ht="15">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="4"/>
@@ -2340,7 +2698,7 @@
       <c r="I47" s="4"/>
       <c r="J47" s="4"/>
     </row>
-    <row r="48" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" ht="15">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="4"/>
@@ -2354,17 +2712,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C17">
-    <cfRule type="cellIs" dxfId="18" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="3" operator="greaterThan">
       <formula>$D$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E17">
-    <cfRule type="cellIs" dxfId="17" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="2" operator="greaterThan">
       <formula>$F$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G17">
-    <cfRule type="cellIs" dxfId="16" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="1" operator="greaterThan">
       <formula>$H$2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2373,22 +2731,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{082C1B9E-BEF4-4D2E-A59E-F7F0A8E0EE98}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2:G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="14.77734375" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" customWidth="1"/>
-    <col min="3" max="10" width="14.77734375" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="10" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2420,7 +2778,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="15">
       <c r="A2" s="6">
         <v>183011218</v>
       </c>
@@ -2456,7 +2814,7 @@
         <v>C+</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="15">
       <c r="A3" s="6">
         <v>173014033</v>
       </c>
@@ -2488,7 +2846,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="15">
       <c r="A4" s="6">
         <v>181014001</v>
       </c>
@@ -2520,7 +2878,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="15">
       <c r="A5" s="6">
         <v>181014051</v>
       </c>
@@ -2552,7 +2910,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="15">
       <c r="A6" s="6">
         <v>181014126</v>
       </c>
@@ -2584,7 +2942,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="15">
       <c r="A7" s="6">
         <v>182014056</v>
       </c>
@@ -2616,7 +2974,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="15">
       <c r="A8" s="6">
         <v>183014070</v>
       </c>
@@ -2652,7 +3010,7 @@
         <v>D</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="15">
       <c r="A9" s="6">
         <v>191014032</v>
       </c>
@@ -2684,7 +3042,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="15">
       <c r="A10" s="6">
         <v>193014009</v>
       </c>
@@ -2720,7 +3078,7 @@
         <v>D</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="15">
       <c r="A11" s="6">
         <v>193014067</v>
       </c>
@@ -2756,7 +3114,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="15">
       <c r="A12" s="6">
         <v>193014071</v>
       </c>
@@ -2792,7 +3150,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="15">
       <c r="A13" s="6">
         <v>193014072</v>
       </c>
@@ -2824,7 +3182,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="15">
       <c r="A14" s="6">
         <v>193014073</v>
       </c>
@@ -2860,7 +3218,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="15">
       <c r="A15" s="6">
         <v>183016002</v>
       </c>
@@ -2892,7 +3250,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="15">
       <c r="A16" s="6">
         <v>192016001</v>
       </c>
@@ -2924,7 +3282,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" ht="15">
       <c r="A17" s="6">
         <v>193016008</v>
       </c>
@@ -2962,12 +3320,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C17">
-    <cfRule type="cellIs" dxfId="15" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="greaterThan">
       <formula>$D$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E17">
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="greaterThan">
       <formula>$F$2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2975,22 +3333,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EAC316A-1F4D-4E67-A257-43105822BFCC}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2:G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="14.77734375" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" customWidth="1"/>
-    <col min="3" max="10" width="14.77734375" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="10" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3022,7 +3380,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="15">
       <c r="A2" s="6">
         <v>183011218</v>
       </c>
@@ -3058,7 +3416,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="15">
       <c r="A3" s="6">
         <v>173014033</v>
       </c>
@@ -3090,7 +3448,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="15">
       <c r="A4" s="6">
         <v>181014001</v>
       </c>
@@ -3122,7 +3480,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="15">
       <c r="A5" s="6">
         <v>181014051</v>
       </c>
@@ -3154,7 +3512,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="15">
       <c r="A6" s="6">
         <v>181014126</v>
       </c>
@@ -3186,7 +3544,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="15">
       <c r="A7" s="6">
         <v>182014056</v>
       </c>
@@ -3222,7 +3580,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="15">
       <c r="A8" s="6">
         <v>183014070</v>
       </c>
@@ -3254,7 +3612,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="15">
       <c r="A9" s="6">
         <v>191014032</v>
       </c>
@@ -3286,7 +3644,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="15">
       <c r="A10" s="6">
         <v>193014009</v>
       </c>
@@ -3318,7 +3676,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="15">
       <c r="A11" s="6">
         <v>193014067</v>
       </c>
@@ -3350,7 +3708,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="15">
       <c r="A12" s="6">
         <v>193014071</v>
       </c>
@@ -3386,7 +3744,7 @@
         <v>B</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="15">
       <c r="A13" s="6">
         <v>193014072</v>
       </c>
@@ -3418,7 +3776,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="15">
       <c r="A14" s="6">
         <v>193014073</v>
       </c>
@@ -3450,7 +3808,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="15">
       <c r="A15" s="6">
         <v>183016002</v>
       </c>
@@ -3482,7 +3840,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="15">
       <c r="A16" s="6">
         <v>192016001</v>
       </c>
@@ -3518,7 +3876,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" ht="15">
       <c r="A17" s="6">
         <v>193016008</v>
       </c>
@@ -3556,12 +3914,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E17">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="greaterThan">
       <formula>$F$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C17">
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="greaterThan">
       <formula>$D$2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3569,23 +3927,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2461B99B-E650-4F8E-B1A3-A4187F7BFC8C}">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="14.77734375" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" customWidth="1"/>
-    <col min="3" max="7" width="14.77734375" customWidth="1"/>
-    <col min="8" max="10" width="14.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="10" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3617,7 +3974,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="15">
       <c r="A2" s="6">
         <v>183011218</v>
       </c>
@@ -3653,7 +4010,7 @@
         <v>D</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="15">
       <c r="A3" s="6">
         <v>173014033</v>
       </c>
@@ -3689,7 +4046,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="15">
       <c r="A4" s="6">
         <v>181014001</v>
       </c>
@@ -3725,7 +4082,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="15">
       <c r="A5" s="6">
         <v>181014051</v>
       </c>
@@ -3761,7 +4118,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="15">
       <c r="A6" s="6">
         <v>181014126</v>
       </c>
@@ -3797,7 +4154,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="15">
       <c r="A7" s="6">
         <v>182014056</v>
       </c>
@@ -3833,7 +4190,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="15">
       <c r="A8" s="6">
         <v>183014070</v>
       </c>
@@ -3869,7 +4226,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="15">
       <c r="A9" s="6">
         <v>191014032</v>
       </c>
@@ -3905,7 +4262,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="15">
       <c r="A10" s="6">
         <v>193014009</v>
       </c>
@@ -3941,7 +4298,7 @@
         <v>C+</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="15">
       <c r="A11" s="6">
         <v>193014067</v>
       </c>
@@ -3977,7 +4334,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="15">
       <c r="A12" s="6">
         <v>193014071</v>
       </c>
@@ -4013,7 +4370,7 @@
         <v>B-</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="15">
       <c r="A13" s="6">
         <v>193014072</v>
       </c>
@@ -4049,7 +4406,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="15">
       <c r="A14" s="6">
         <v>193014073</v>
       </c>
@@ -4085,7 +4442,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="15">
       <c r="A15" s="6">
         <v>183016002</v>
       </c>
@@ -4121,7 +4478,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="15">
       <c r="A16" s="6">
         <v>192016001</v>
       </c>
@@ -4157,7 +4514,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" ht="15">
       <c r="A17" s="6">
         <v>193016008</v>
       </c>
@@ -4199,23 +4556,23 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:P17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" customWidth="1"/>
-    <col min="3" max="15" width="14.6640625" customWidth="1"/>
-    <col min="16" max="16" width="14.6640625" style="9" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="15" width="14.7109375" customWidth="1"/>
+    <col min="16" max="16" width="14.7109375" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="15.95" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4265,7 +4622,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" ht="15" customHeight="1">
       <c r="A2" s="6">
         <v>183011218</v>
       </c>
@@ -4315,7 +4672,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" ht="15" customHeight="1">
       <c r="A3" s="6">
         <v>173014033</v>
       </c>
@@ -4359,7 +4716,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" ht="15" customHeight="1">
       <c r="A4" s="6">
         <v>181014001</v>
       </c>
@@ -4403,7 +4760,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" ht="15" customHeight="1">
       <c r="A5" s="6">
         <v>181014051</v>
       </c>
@@ -4447,7 +4804,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" ht="15" customHeight="1">
       <c r="A6" s="6">
         <v>181014126</v>
       </c>
@@ -4495,7 +4852,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" ht="15" customHeight="1">
       <c r="A7" s="6">
         <v>182014056</v>
       </c>
@@ -4543,7 +4900,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" ht="15" customHeight="1">
       <c r="A8" s="6">
         <v>183014070</v>
       </c>
@@ -4593,7 +4950,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" ht="15" customHeight="1">
       <c r="A9" s="6">
         <v>191014032</v>
       </c>
@@ -4637,7 +4994,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" ht="15" customHeight="1">
       <c r="A10" s="6">
         <v>193014009</v>
       </c>
@@ -4687,7 +5044,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" ht="15" customHeight="1">
       <c r="A11" s="6">
         <v>193014067</v>
       </c>
@@ -4735,7 +5092,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" ht="15" customHeight="1">
       <c r="A12" s="6">
         <v>193014071</v>
       </c>
@@ -4789,7 +5146,7 @@
         <v>D</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" ht="15" customHeight="1">
       <c r="A13" s="6">
         <v>193014072</v>
       </c>
@@ -4833,7 +5190,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" ht="15" customHeight="1">
       <c r="A14" s="6">
         <v>193014073</v>
       </c>
@@ -4881,7 +5238,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" ht="15" customHeight="1">
       <c r="A15" s="6">
         <v>183016002</v>
       </c>
@@ -4925,7 +5282,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" ht="15" customHeight="1">
       <c r="A16" s="6">
         <v>192016001</v>
       </c>
@@ -4973,7 +5330,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" ht="15" customHeight="1">
       <c r="A17" s="6">
         <v>193016008</v>
       </c>
@@ -5025,27 +5382,27 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C17">
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="greaterThan">
       <formula>$D$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E17">
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="greaterThan">
       <formula>$F$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G17">
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="greaterThan">
       <formula>$H$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I17">
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="greaterThan">
       <formula>$J$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K17">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
       <formula>$L$2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5053,22 +5410,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01230E4E-9F21-464B-AB8D-C05858C1812B}">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R19"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="14.77734375" customWidth="1"/>
-    <col min="2" max="2" width="30.77734375" customWidth="1"/>
-    <col min="3" max="18" width="14.77734375" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="18" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5124,7 +5481,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="15">
       <c r="A2" s="6">
         <v>183011218</v>
       </c>
@@ -5184,7 +5541,7 @@
         <v>B+</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="15">
       <c r="A3" s="6">
         <v>173014033</v>
       </c>
@@ -5232,7 +5589,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="15">
       <c r="A4" s="6">
         <v>181014001</v>
       </c>
@@ -5280,7 +5637,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="15">
       <c r="A5" s="6">
         <v>181014051</v>
       </c>
@@ -5328,7 +5685,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="15">
       <c r="A6" s="6">
         <v>181014126</v>
       </c>
@@ -5376,7 +5733,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="15">
       <c r="A7" s="6">
         <v>182014056</v>
       </c>
@@ -5434,7 +5791,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="15">
       <c r="A8" s="6">
         <v>183014070</v>
       </c>
@@ -5494,7 +5851,7 @@
         <v>C+</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="15">
       <c r="A9" s="6">
         <v>191014032</v>
       </c>
@@ -5542,7 +5899,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="15">
       <c r="A10" s="6">
         <v>193014009</v>
       </c>
@@ -5600,7 +5957,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" ht="15">
       <c r="A11" s="6">
         <v>193014067</v>
       </c>
@@ -5658,7 +6015,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" ht="15">
       <c r="A12" s="6">
         <v>193014071</v>
       </c>
@@ -5718,7 +6075,7 @@
         <v>C+</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" ht="15">
       <c r="A13" s="6">
         <v>193014072</v>
       </c>
@@ -5766,7 +6123,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" ht="15">
       <c r="A14" s="6">
         <v>193014073</v>
       </c>
@@ -5824,7 +6181,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" ht="15">
       <c r="A15" s="6">
         <v>183016002</v>
       </c>
@@ -5872,7 +6229,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" ht="15">
       <c r="A16" s="6">
         <v>192016001</v>
       </c>
@@ -5932,7 +6289,7 @@
         <v>B+</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" ht="15">
       <c r="A17" s="6">
         <v>193016008</v>
       </c>
@@ -5992,33 +6349,33 @@
         <v>B+</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18">
       <c r="R19" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="C2:C17">
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
       <formula>$D$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E17">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
       <formula>$F$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G17">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
       <formula>$H$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I17">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>$J$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K17">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>$L$2</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>